<commit_message>
Add BCF GWAS + Harmonization + Heatmaps + prepruned T1D
</commit_message>
<xml_diff>
--- a/1_GWAS Downloading and Harmonization/Data/GWAS traits tables/gwas_traits.xlsx
+++ b/1_GWAS Downloading and Harmonization/Data/GWAS traits tables/gwas_traits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7474c0e581ffbaf/Umich/lab/Stephen CJ Parker/T1D soft clustering/GWAS summary stats/GWAS traits tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_9A5207BB3979FF691316C2B5EB87A551FC8E51C0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C09693C6-9C84-8C41-8221-0238A97150ED}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="11_9A5207BB3979FF691316C2B5EB87A551FC8E51C0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA9E09CB-3DD6-424A-8B57-58A1B10CE079}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="2680" windowWidth="21400" windowHeight="15700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6160" yWindow="1920" windowWidth="21400" windowHeight="15700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main_gwas" sheetId="1" r:id="rId1"/>
@@ -7152,6 +7152,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7477,8 +7481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F751"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22513,11 +22517,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -23530,7 +23537,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>